<commit_message>
feat analisis modelos RW
</commit_message>
<xml_diff>
--- a/Inventor/Pesos EyasSat.xlsx
+++ b/Inventor/Pesos EyasSat.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Documents\TDG_Sebastian\TDG_ReactionWheelsUnloading\Inventor\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Personal\Documents\GitHub\TDG_ReactionWheelsUnloading\Inventor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B6F6D33-7108-4A8D-9D5A-58E2F45A61AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B0E5CA3-677B-4760-BB77-0B0327991623}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{D8D42D20-FFF3-457A-BB76-F454978782DD}"/>
+    <workbookView xWindow="-25320" yWindow="3660" windowWidth="25440" windowHeight="15390" xr2:uid="{D8D42D20-FFF3-457A-BB76-F454978782DD}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,17 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -515,7 +526,7 @@
   <dimension ref="A1:E46"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="D43" sqref="D43"/>
+      <selection activeCell="A49" sqref="A49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>